<commit_message>
fix approach_3 Spanish results
</commit_message>
<xml_diff>
--- a/status_amz.xlsx
+++ b/status_amz.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2350" windowHeight="4340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>dir_name</t>
   </si>
@@ -65,8 +65,20 @@
     <t>labse</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">translated EN ds to ES using </t>
+    <t>translation_transformer_Helsinki/LABSE</t>
+  </si>
+  <si>
+    <t>translation_transformer_Helsinki/bert_base_es_cased</t>
+  </si>
+  <si>
+    <t>bert_base_es_cased</t>
+  </si>
+  <si>
+    <t>approach_3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Translated EN ds to ES using </t>
     </r>
     <r>
       <rPr>
@@ -116,17 +128,8 @@
     </r>
   </si>
   <si>
-    <t>translation_transformer_Helsinki/LABSE</t>
-  </si>
-  <si>
-    <t>translation_transformer_Helsinki/bert_base_es_cased</t>
-  </si>
-  <si>
-    <t>bert_base_es_cased</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">translated EN ds to ES using </t>
+    <r>
+      <t xml:space="preserve">Translated EN ds to ES using </t>
     </r>
     <r>
       <rPr>
@@ -176,14 +179,105 @@
     </r>
   </si>
   <si>
-    <t>approach_3</t>
+    <r>
+      <t>Train an English model using</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> roberta-base.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Create synthetic labels using the English model, for the Spanish dataset ( translation using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Helsinki, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">embedded using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>roberta-base</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).
+Then train a model using native Spanish dataset with the  synthetic labels (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">using bert-base-es-cased . </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Predict using native Spanish val dataset.</t>
+    </r>
+  </si>
+  <si>
+    <t>roberta-base and bert-base-es-cased</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +288,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -266,18 +367,7 @@
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -286,8 +376,43 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="5"/>
+      </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="5"/>
+      </top>
+      <bottom style="medium">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="5"/>
+      </right>
+      <top style="medium">
+        <color theme="5"/>
+      </top>
+      <bottom style="medium">
+        <color theme="5"/>
       </bottom>
       <diagonal/>
     </border>
@@ -295,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -306,12 +431,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,7 +725,7 @@
   <dimension ref="F6:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,7 +738,7 @@
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -676,10 +806,10 @@
     </row>
     <row r="8" spans="6:15" ht="58" x14ac:dyDescent="0.35">
       <c r="F8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H8" s="5">
         <v>80000</v>
@@ -706,10 +836,10 @@
     </row>
     <row r="9" spans="6:15" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F9" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="9">
         <v>80000</v>
@@ -730,14 +860,39 @@
         <v>0.92900000000000005</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O9" s="10"/>
     </row>
-    <row r="10" spans="6:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="6:15" ht="131" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F10" s="11" t="s">
-        <v>18</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="13">
+        <v>8000</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2000</v>
+      </c>
+      <c r="J10" s="9">
+        <v>2000</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0.99</v>
+      </c>
+      <c r="L10" s="13">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="M10" s="13">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>